<commit_message>
update profile and timesheet
</commit_message>
<xml_diff>
--- a/stuff/timesheet/Trainee Timesheet 2020.xlsx
+++ b/stuff/timesheet/Trainee Timesheet 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skw9h\git\novus\stuff\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1545CE2C-EABA-42D8-A260-31EB361AA998}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FC0401-60E3-4540-AEF8-4EA1EE6F0833}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="36">
   <si>
     <t>Monday</t>
   </si>
@@ -132,16 +132,19 @@
     <t>09:30 to 15:00</t>
   </si>
   <si>
-    <t>if/else and for loops</t>
-  </si>
-  <si>
     <t>10:00 to 16:00</t>
   </si>
   <si>
     <t>09:00 to 16:00</t>
   </si>
   <si>
-    <t>4 pillars of OOP</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Basic Java</t>
+  </si>
+  <si>
+    <t>OOP</t>
   </si>
 </sst>
 </file>
@@ -773,7 +776,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -819,7 +822,7 @@
       </c>
       <c r="H2" s="18">
         <f>SUM(H7,H14,H21,H28,H35,H42,H49,H56,H63,H70)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -951,10 +954,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F10" s="24"/>
     </row>
@@ -969,10 +972,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" s="24"/>
     </row>
@@ -983,9 +986,15 @@
       <c r="B12" s="13">
         <v>43852</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:9" ht="16" thickBot="1">
@@ -1028,7 +1037,7 @@
       </c>
       <c r="H14" s="18">
         <f>SUM(C10:C14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3250,12 +3259,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3391,15 +3397,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DF210E8-F54B-40DF-8EF5-311E887C878B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576F1911-9305-4369-B84A-D752319CC3E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3423,10 +3433,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576F1911-9305-4369-B84A-D752319CC3E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DF210E8-F54B-40DF-8EF5-311E887C878B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated timesheet and profile
</commit_message>
<xml_diff>
--- a/stuff/timesheet/Trainee Timesheet 2020.xlsx
+++ b/stuff/timesheet/Trainee Timesheet 2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skw9h\git\novus\stuff\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043448A5-E573-46D2-AA19-762548278C39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A0DE84D-D6FA-46EA-88FE-05ACA69E91F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,11 +21,14 @@
     <sheet name="Nov 2019" sheetId="5" r:id="rId6"/>
     <sheet name="Dec 2019" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -36,138 +39,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="45">
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>In training? Enter either 1 (yes) or 0 (no)</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>OVERALL TOTAL</t>
+  </si>
   <si>
     <t>Monday</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Tuesday</t>
   </si>
   <si>
+    <t>09:30 to 16:30</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>09:30 to 16:00</t>
+  </si>
+  <si>
+    <t>Interview Skills</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>09:30 to 15:00</t>
+  </si>
+  <si>
+    <t>Presentation Skills</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>10:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Basic Java</t>
+  </si>
+  <si>
+    <t>09:00 to 16:00</t>
+  </si>
+  <si>
+    <t>OOP</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>9:30 to 16:00</t>
+  </si>
+  <si>
+    <t>Scrum Cycle</t>
+  </si>
+  <si>
+    <t>Testing Theory</t>
+  </si>
+  <si>
+    <t>BAE Systems</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Test/Git</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>GIT/SOAP</t>
+  </si>
+  <si>
+    <t>SOAP/REST</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>SELENIUM</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
     <t>Wedneday</t>
   </si>
   <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date </t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>In training? Enter either 1 (yes) or 0 (no)</t>
-  </si>
-  <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 8</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
-    <t>Week 10</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>09:30 to 16:00</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Introduction</t>
-  </si>
-  <si>
-    <t>Presentation Skills</t>
-  </si>
-  <si>
-    <t>Interview Skills</t>
-  </si>
-  <si>
-    <t>OVERALL TOTAL</t>
-  </si>
-  <si>
-    <t>09:30 to 16:30</t>
-  </si>
-  <si>
-    <t>09:30 to 15:00</t>
-  </si>
-  <si>
-    <t>10:00 to 16:00</t>
-  </si>
-  <si>
-    <t>09:00 to 16:00</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Basic Java</t>
-  </si>
-  <si>
-    <t>OOP</t>
-  </si>
-  <si>
-    <t>9:30 to 16:00</t>
-  </si>
-  <si>
-    <t>Scrum Cycle</t>
-  </si>
-  <si>
-    <t>BAE Systems</t>
-  </si>
-  <si>
-    <t>Testing Theory</t>
-  </si>
-  <si>
-    <t>Jenkins</t>
-  </si>
-  <si>
-    <t>Test/Git</t>
-  </si>
-  <si>
-    <t>GIT/SOAP</t>
-  </si>
-  <si>
-    <t>SOAP/REST</t>
   </si>
 </sst>
 </file>
@@ -465,16 +471,16 @@
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Currency" xfId="11" builtinId="4"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -814,42 +820,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9464A641-8300-D948-AF69-2A933AAD673F}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="18" style="11" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="11" customWidth="1"/>
     <col min="3" max="3" width="39" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="11" customWidth="1"/>
     <col min="5" max="5" width="24" style="11" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" thickBot="1">
+    <row r="1" spans="1:9" ht="15.95" thickBot="1">
       <c r="A1" s="9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.95" thickBot="1">
+      <c r="A2" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" thickBot="1">
-      <c r="A2" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -857,16 +863,16 @@
       <c r="E2" s="10"/>
       <c r="F2" s="22"/>
       <c r="G2" s="26" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="H2" s="17">
         <f>SUM(H7,H14,H21,H28,H35,H42,H49,H56,H63,H70)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" s="13">
         <v>43843</v>
@@ -875,22 +881,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="15"/>
       <c r="H3" s="29">
         <f xml:space="preserve"> 20*H2</f>
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B4" s="13">
         <v>43844</v>
@@ -899,16 +905,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="13">
         <v>43845</v>
@@ -917,16 +923,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:9" ht="16" thickBot="1">
+    <row r="6" spans="1:9" ht="15.95" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B6" s="13">
         <v>43846</v>
@@ -935,16 +941,16 @@
         <v>1</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:9" ht="16" thickBot="1">
+    <row r="7" spans="1:9" ht="15.95" thickBot="1">
       <c r="A7" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B7" s="21">
         <v>43847</v>
@@ -953,14 +959,14 @@
         <v>1</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7" s="17">
         <f>SUM(C2:C7)</f>
@@ -977,7 +983,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="12" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -987,7 +993,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B10" s="13">
         <v>43850</v>
@@ -996,16 +1002,16 @@
         <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B11" s="13">
         <v>43851</v>
@@ -1014,16 +1020,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B12" s="13">
         <v>43852</v>
@@ -1032,16 +1038,16 @@
         <v>1</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F12" s="23"/>
     </row>
-    <row r="13" spans="1:9" ht="16" thickBot="1">
+    <row r="13" spans="1:9" ht="15.95" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B13" s="13">
         <v>43853</v>
@@ -1050,16 +1056,16 @@
         <v>0</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F13" s="23"/>
     </row>
-    <row r="14" spans="1:9" ht="16" thickBot="1">
+    <row r="14" spans="1:9" ht="15.95" thickBot="1">
       <c r="A14" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B14" s="21">
         <v>43854</v>
@@ -1068,14 +1074,14 @@
         <v>0</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H14" s="17">
         <f>SUM(C10:C14)</f>
@@ -1092,7 +1098,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="12" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1102,7 +1108,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B17" s="13">
         <v>43857</v>
@@ -1111,16 +1117,16 @@
         <v>1</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B18" s="13">
         <v>43858</v>
@@ -1129,16 +1135,16 @@
         <v>1</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B19" s="13">
         <v>43859</v>
@@ -1147,16 +1153,16 @@
         <v>1</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F19" s="23"/>
     </row>
-    <row r="20" spans="1:8" ht="16" thickBot="1">
+    <row r="20" spans="1:8" ht="15.95" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B20" s="13">
         <v>43860</v>
@@ -1165,16 +1171,16 @@
         <v>0</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F20" s="23"/>
     </row>
-    <row r="21" spans="1:8" ht="16" thickBot="1">
+    <row r="21" spans="1:8" ht="15.95" thickBot="1">
       <c r="A21" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B21" s="21">
         <v>43861</v>
@@ -1183,14 +1189,14 @@
         <v>0</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H21" s="17">
         <f>SUM(C17:C21)</f>
@@ -1207,7 +1213,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1217,7 +1223,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B24" s="13">
         <v>43864</v>
@@ -1226,16 +1232,16 @@
         <v>1</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B25" s="13">
         <v>43865</v>
@@ -1244,16 +1250,16 @@
         <v>0</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B26" s="13">
         <v>43866</v>
@@ -1262,16 +1268,16 @@
         <v>1</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="16" thickBot="1">
+    <row r="27" spans="1:8" ht="15.95" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B27" s="13">
         <v>43867</v>
@@ -1280,16 +1286,16 @@
         <v>0</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F27" s="23"/>
     </row>
-    <row r="28" spans="1:8" ht="16" thickBot="1">
+    <row r="28" spans="1:8" ht="15.95" thickBot="1">
       <c r="A28" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B28" s="21">
         <v>43868</v>
@@ -1298,14 +1304,14 @@
         <v>0</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H28" s="17">
         <f>SUM(C24:C28)</f>
@@ -1322,7 +1328,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="12" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1332,7 +1338,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B31" s="13">
         <v>43871</v>
@@ -1341,34 +1347,34 @@
         <v>1</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F31" s="23"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B32" s="13">
         <v>43872</v>
       </c>
       <c r="C32" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B33" s="13">
         <v>43873</v>
@@ -1377,16 +1383,16 @@
         <v>1</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F33" s="23"/>
     </row>
-    <row r="34" spans="1:8" ht="16" thickBot="1">
+    <row r="34" spans="1:8" ht="15.95" thickBot="1">
       <c r="A34" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B34" s="13">
         <v>43874</v>
@@ -1395,16 +1401,16 @@
         <v>0</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F34" s="23"/>
     </row>
-    <row r="35" spans="1:8" ht="16" thickBot="1">
+    <row r="35" spans="1:8" ht="15.95" thickBot="1">
       <c r="A35" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B35" s="21">
         <v>43875</v>
@@ -1413,18 +1419,18 @@
         <v>0</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H35" s="17">
         <f>SUM(C31:C35)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1437,7 +1443,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="12" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -1447,7 +1453,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B38" s="13">
         <v>43878</v>
@@ -1456,16 +1462,16 @@
         <v>1</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F38" s="23"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B39" s="13">
         <v>43879</v>
@@ -1474,34 +1480,34 @@
         <v>1</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F39" s="23"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B40" s="13">
         <v>43880</v>
       </c>
       <c r="C40" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>21</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F40" s="23"/>
     </row>
-    <row r="41" spans="1:8" ht="16" thickBot="1">
+    <row r="41" spans="1:8" ht="15.95" thickBot="1">
       <c r="A41" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B41" s="13">
         <v>43881</v>
@@ -1510,16 +1516,16 @@
         <v>0</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F41" s="23"/>
     </row>
-    <row r="42" spans="1:8" ht="16" thickBot="1">
+    <row r="42" spans="1:8" ht="15.95" thickBot="1">
       <c r="A42" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B42" s="21">
         <v>43882</v>
@@ -1528,18 +1534,18 @@
         <v>0</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F42" s="24"/>
       <c r="G42" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H42" s="17">
         <f>SUM(C38:C42)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1552,7 +1558,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="12" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -1562,69 +1568,99 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B45" s="13">
         <v>43885</v>
       </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
+      <c r="C45" s="10">
+        <v>1</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="F45" s="23"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B46" s="13">
         <v>43886</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="C46" s="10">
+        <v>1</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="F46" s="23"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B47" s="13">
         <v>43887</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
+      <c r="C47" s="10">
+        <v>0</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="F47" s="23"/>
     </row>
-    <row r="48" spans="1:8" ht="16" thickBot="1">
+    <row r="48" spans="1:8" ht="15.95" thickBot="1">
       <c r="A48" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B48" s="13">
         <v>43888</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
+      <c r="C48" s="10">
+        <v>0</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="F48" s="23"/>
     </row>
-    <row r="49" spans="1:8" ht="16" thickBot="1">
+    <row r="49" spans="1:8" ht="15.95" thickBot="1">
       <c r="A49" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B49" s="21">
         <v>43889</v>
       </c>
-      <c r="C49" s="20"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
+      <c r="C49" s="20">
+        <v>0</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>8</v>
+      </c>
       <c r="F49" s="24"/>
       <c r="G49" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H49" s="17">
         <f>SUM(C45:C49)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1637,7 +1673,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="12" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -1647,7 +1683,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B52" s="13">
         <v>43892</v>
@@ -1659,7 +1695,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B53" s="13">
         <v>43893</v>
@@ -1671,7 +1707,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B54" s="13">
         <v>43894</v>
@@ -1681,9 +1717,9 @@
       <c r="E54" s="13"/>
       <c r="F54" s="23"/>
     </row>
-    <row r="55" spans="1:8" ht="16" thickBot="1">
+    <row r="55" spans="1:8" ht="15.95" thickBot="1">
       <c r="A55" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B55" s="13">
         <v>43895</v>
@@ -1693,9 +1729,9 @@
       <c r="E55" s="13"/>
       <c r="F55" s="23"/>
     </row>
-    <row r="56" spans="1:8" ht="16" thickBot="1">
+    <row r="56" spans="1:8" ht="15.95" thickBot="1">
       <c r="A56" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B56" s="21">
         <v>43896</v>
@@ -1705,7 +1741,7 @@
       <c r="E56" s="21"/>
       <c r="F56" s="24"/>
       <c r="G56" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H56" s="17">
         <f>SUM(C52:C56)</f>
@@ -1722,7 +1758,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="12" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -1732,7 +1768,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B59" s="13">
         <v>43899</v>
@@ -1744,7 +1780,7 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B60" s="13">
         <v>43900</v>
@@ -1756,7 +1792,7 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B61" s="13">
         <v>43901</v>
@@ -1766,9 +1802,9 @@
       <c r="E61" s="13"/>
       <c r="F61" s="23"/>
     </row>
-    <row r="62" spans="1:8" ht="16" thickBot="1">
+    <row r="62" spans="1:8" ht="15.95" thickBot="1">
       <c r="A62" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B62" s="13">
         <v>43902</v>
@@ -1778,9 +1814,9 @@
       <c r="E62" s="13"/>
       <c r="F62" s="23"/>
     </row>
-    <row r="63" spans="1:8" ht="16" thickBot="1">
+    <row r="63" spans="1:8" ht="15.95" thickBot="1">
       <c r="A63" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B63" s="21">
         <v>43903</v>
@@ -1790,7 +1826,7 @@
       <c r="E63" s="21"/>
       <c r="F63" s="24"/>
       <c r="G63" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H63" s="17">
         <f>SUM(C59:C63)</f>
@@ -1807,7 +1843,7 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="12" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -1817,7 +1853,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B66" s="13">
         <v>43906</v>
@@ -1829,7 +1865,7 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B67" s="13">
         <v>43907</v>
@@ -1841,7 +1877,7 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B68" s="13">
         <v>43908</v>
@@ -1851,9 +1887,9 @@
       <c r="E68" s="13"/>
       <c r="F68" s="23"/>
     </row>
-    <row r="69" spans="1:8" ht="16" thickBot="1">
+    <row r="69" spans="1:8" ht="15.95" thickBot="1">
       <c r="A69" s="10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B69" s="13">
         <v>43909</v>
@@ -1863,9 +1899,9 @@
       <c r="E69" s="13"/>
       <c r="F69" s="23"/>
     </row>
-    <row r="70" spans="1:8" ht="16" thickBot="1">
+    <row r="70" spans="1:8" ht="15.95" thickBot="1">
       <c r="A70" s="20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B70" s="21">
         <v>43910</v>
@@ -1875,7 +1911,7 @@
       <c r="E70" s="21"/>
       <c r="F70" s="24"/>
       <c r="G70" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H70" s="17">
         <f>SUM(C66:C70)</f>
@@ -1901,28 +1937,28 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>43647</v>
@@ -1930,7 +1966,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>43648</v>
@@ -1938,7 +1974,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4">
         <v>43649</v>
@@ -1946,7 +1982,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>43650</v>
@@ -1954,7 +1990,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>43651</v>
@@ -1968,7 +2004,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4">
         <v>43654</v>
@@ -1976,7 +2012,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>43655</v>
@@ -1984,7 +2020,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4">
         <v>43656</v>
@@ -1992,7 +2028,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4">
         <v>43657</v>
@@ -2000,7 +2036,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
         <v>43658</v>
@@ -2014,7 +2050,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4">
         <v>43661</v>
@@ -2022,7 +2058,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4">
         <v>43662</v>
@@ -2030,7 +2066,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4">
         <v>43663</v>
@@ -2038,7 +2074,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4">
         <v>43664</v>
@@ -2046,7 +2082,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4">
         <v>43665</v>
@@ -2060,7 +2096,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B25" s="4">
         <v>43668</v>
@@ -2068,7 +2104,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B26" s="4">
         <v>43669</v>
@@ -2076,7 +2112,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4">
         <v>43670</v>
@@ -2084,7 +2120,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B28" s="4">
         <v>43671</v>
@@ -2092,7 +2128,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B29" s="4">
         <v>43672</v>
@@ -2106,7 +2142,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B32" s="4">
         <v>43675</v>
@@ -2114,7 +2150,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B33" s="4">
         <v>43676</v>
@@ -2122,7 +2158,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B34" s="4">
         <v>43677</v>
@@ -2131,7 +2167,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="C35" s="7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D35" s="8">
         <f>SUM(C2:C34)</f>
@@ -2167,27 +2203,27 @@
       <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>43678</v>
@@ -2195,7 +2231,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4">
         <v>43679</v>
@@ -2209,7 +2245,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>43682</v>
@@ -2217,7 +2253,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4">
         <v>43683</v>
@@ -2225,7 +2261,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4">
         <v>43684</v>
@@ -2233,7 +2269,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4">
         <v>43685</v>
@@ -2241,7 +2277,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4">
         <v>43686</v>
@@ -2255,7 +2291,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B15" s="4">
         <v>43689</v>
@@ -2263,7 +2299,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B16" s="4">
         <v>43690</v>
@@ -2271,7 +2307,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B17" s="4">
         <v>43691</v>
@@ -2279,7 +2315,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4">
         <v>43692</v>
@@ -2287,7 +2323,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
         <v>43693</v>
@@ -2301,7 +2337,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B22" s="4">
         <v>43696</v>
@@ -2309,7 +2345,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B23" s="4">
         <v>43697</v>
@@ -2317,7 +2353,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B24" s="4">
         <v>43698</v>
@@ -2325,7 +2361,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B25" s="4">
         <v>43699</v>
@@ -2333,7 +2369,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B26" s="4">
         <v>43700</v>
@@ -2347,7 +2383,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B29" s="4">
         <v>43703</v>
@@ -2355,7 +2391,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B30" s="4">
         <v>43704</v>
@@ -2363,7 +2399,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B31" s="4">
         <v>43705</v>
@@ -2371,7 +2407,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B32" s="4">
         <v>43706</v>
@@ -2379,7 +2415,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B33" s="4">
         <v>43707</v>
@@ -2389,7 +2425,7 @@
     <row r="34" spans="1:4">
       <c r="B34" s="4"/>
       <c r="C34" s="7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D34" s="8">
         <f>SUM(C2:C33)</f>
@@ -2419,27 +2455,27 @@
       <selection activeCell="C33" sqref="C33:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>43710</v>
@@ -2447,7 +2483,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>43711</v>
@@ -2455,7 +2491,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4">
         <v>43712</v>
@@ -2463,7 +2499,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>43713</v>
@@ -2471,7 +2507,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>43714</v>
@@ -2485,7 +2521,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4">
         <v>43717</v>
@@ -2493,7 +2529,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>43718</v>
@@ -2501,7 +2537,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4">
         <v>43719</v>
@@ -2509,7 +2545,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4">
         <v>43720</v>
@@ -2517,7 +2553,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
         <v>43721</v>
@@ -2531,7 +2567,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4">
         <v>43724</v>
@@ -2539,7 +2575,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4">
         <v>43725</v>
@@ -2547,7 +2583,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4">
         <v>43726</v>
@@ -2555,7 +2591,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4">
         <v>43727</v>
@@ -2563,7 +2599,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4">
         <v>43728</v>
@@ -2577,7 +2613,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B25" s="4">
         <v>43731</v>
@@ -2585,7 +2621,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B26" s="4">
         <v>43732</v>
@@ -2593,7 +2629,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4">
         <v>43733</v>
@@ -2601,7 +2637,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B28" s="4">
         <v>43734</v>
@@ -2609,7 +2645,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B29" s="4">
         <v>43735</v>
@@ -2623,7 +2659,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B32" s="4">
         <v>43738</v>
@@ -2633,7 +2669,7 @@
     <row r="33" spans="2:4">
       <c r="B33" s="4"/>
       <c r="C33" s="7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D33" s="8">
         <f>SUM(C3:C32)</f>
@@ -2669,27 +2705,27 @@
       <selection activeCell="C35" sqref="C35:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4">
         <v>43739</v>
@@ -2697,7 +2733,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B5" s="4">
         <v>43740</v>
@@ -2705,7 +2741,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4">
         <v>43741</v>
@@ -2713,7 +2749,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>43742</v>
@@ -2727,7 +2763,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4">
         <v>43745</v>
@@ -2735,7 +2771,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4">
         <v>43746</v>
@@ -2743,7 +2779,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B12" s="4">
         <v>43747</v>
@@ -2751,7 +2787,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B13" s="4">
         <v>43748</v>
@@ -2759,7 +2795,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B14" s="4">
         <v>43749</v>
@@ -2773,7 +2809,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B17" s="4">
         <v>43752</v>
@@ -2781,7 +2817,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4">
         <v>43753</v>
@@ -2789,7 +2825,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4">
         <v>43754</v>
@@ -2797,7 +2833,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4">
         <v>43755</v>
@@ -2805,7 +2841,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4">
         <v>43756</v>
@@ -2819,7 +2855,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B24" s="4">
         <v>43759</v>
@@ -2827,7 +2863,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B25" s="4">
         <v>43760</v>
@@ -2835,7 +2871,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B26" s="4">
         <v>43761</v>
@@ -2843,7 +2879,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B27" s="4">
         <v>43762</v>
@@ -2851,7 +2887,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B28" s="4">
         <v>43763</v>
@@ -2865,7 +2901,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B31" s="4">
         <v>43766</v>
@@ -2873,7 +2909,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B32" s="4">
         <v>43767</v>
@@ -2881,7 +2917,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B33" s="4">
         <v>43768</v>
@@ -2889,7 +2925,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B34" s="4">
         <v>43769</v>
@@ -2898,7 +2934,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="C35" s="7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D35" s="8">
         <f>SUM(C2:C34)</f>
@@ -2928,27 +2964,27 @@
       <selection activeCell="C33" sqref="C33:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4">
         <v>43770</v>
@@ -2962,7 +2998,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B7" s="4">
         <v>43773</v>
@@ -2970,7 +3006,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>43774</v>
@@ -2978,7 +3014,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4">
         <v>43775</v>
@@ -2986,7 +3022,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B10" s="4">
         <v>43776</v>
@@ -2994,7 +3030,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
         <v>43777</v>
@@ -3008,7 +3044,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4">
         <v>43780</v>
@@ -3016,7 +3052,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4">
         <v>43781</v>
@@ -3024,7 +3060,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4">
         <v>43782</v>
@@ -3032,7 +3068,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>43783</v>
@@ -3040,7 +3076,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B18" s="4">
         <v>43784</v>
@@ -3054,7 +3090,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B21" s="4">
         <v>43787</v>
@@ -3062,7 +3098,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B22" s="4">
         <v>43788</v>
@@ -3070,7 +3106,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B23" s="4">
         <v>43789</v>
@@ -3078,7 +3114,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B24" s="4">
         <v>43790</v>
@@ -3086,7 +3122,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B25" s="4">
         <v>43791</v>
@@ -3100,7 +3136,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B28" s="4">
         <v>43794</v>
@@ -3108,7 +3144,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B29" s="4">
         <v>43795</v>
@@ -3116,7 +3152,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B30" s="4">
         <v>43796</v>
@@ -3124,7 +3160,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B31" s="4">
         <v>43797</v>
@@ -3132,7 +3168,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B32" s="4">
         <v>43798</v>
@@ -3142,7 +3178,7 @@
     <row r="33" spans="2:4">
       <c r="B33" s="4"/>
       <c r="C33" s="7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D33" s="8">
         <f>SUM(C2:C32)</f>
@@ -3173,27 +3209,27 @@
       <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>43801</v>
@@ -3201,7 +3237,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>43802</v>
@@ -3209,7 +3245,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4">
         <v>43803</v>
@@ -3217,7 +3253,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>43804</v>
@@ -3225,7 +3261,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>43805</v>
@@ -3239,7 +3275,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4">
         <v>43808</v>
@@ -3247,7 +3283,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>43809</v>
@@ -3255,7 +3291,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4">
         <v>43810</v>
@@ -3263,7 +3299,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4">
         <v>43811</v>
@@ -3271,7 +3307,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
         <v>43812</v>
@@ -3285,7 +3321,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4">
         <v>43815</v>
@@ -3293,7 +3329,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4">
         <v>43816</v>
@@ -3301,7 +3337,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4">
         <v>43817</v>
@@ -3309,7 +3345,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4">
         <v>43818</v>
@@ -3317,7 +3353,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4">
         <v>43819</v>
@@ -3331,7 +3367,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B25" s="4">
         <v>43822</v>
@@ -3339,7 +3375,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B26" s="4">
         <v>43823</v>
@@ -3347,7 +3383,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4">
         <v>43824</v>
@@ -3355,7 +3391,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B28" s="4">
         <v>43825</v>
@@ -3363,7 +3399,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B29" s="4">
         <v>43826</v>
@@ -3377,7 +3413,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B32" s="4">
         <v>43829</v>
@@ -3385,7 +3421,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B33" s="4">
         <v>43830</v>
@@ -3395,7 +3431,7 @@
     <row r="34" spans="1:4">
       <c r="B34" s="4"/>
       <c r="C34" s="7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D34" s="8">
         <f>SUM(C2:C33)</f>
@@ -3421,15 +3457,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E7FA2392B506B44B1E10B8C7B7E4338" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c8af6b3d6ac204ec2ed4b0f9ca7edc5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="808f2f0d-c9e7-4164-b92e-8f0c1346b995" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b9069dad3d8e874012dc6d49fc7d327" ns2:_="">
     <xsd:import namespace="808f2f0d-c9e7-4164-b92e-8f0c1346b995"/>
@@ -3561,6 +3588,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3568,36 +3604,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DF210E8-F54B-40DF-8EF5-311E887C878B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE7D9017-268A-4AE7-8A8E-7D88AD02F713}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE7D9017-268A-4AE7-8A8E-7D88AD02F713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="808f2f0d-c9e7-4164-b92e-8f0c1346b995"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DF210E8-F54B-40DF-8EF5-311E887C878B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576F1911-9305-4369-B84A-D752319CC3E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576F1911-9305-4369-B84A-D752319CC3E4}"/>
 </file>
</xml_diff>